<commit_message>
Christos completed his skills
</commit_message>
<xml_diff>
--- a/documentation/internal/SkillsMatrix.xlsx
+++ b/documentation/internal/SkillsMatrix.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="15315" windowHeight="11055" activeTab="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="64">
   <si>
     <t>Group 1:</t>
   </si>
@@ -207,16 +207,13 @@
   </si>
   <si>
     <t>MS Project (Gantt charts)</t>
-  </si>
-  <si>
-    <t>t1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,11 +462,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -548,7 +540,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -583,7 +574,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -759,31 +749,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A6:C17"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
     <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" ht="26.25">
       <c r="B6" s="25" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="25"/>
     </row>
-    <row r="7" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" ht="26.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" ht="26.25">
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -791,7 +781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" ht="26.25">
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
@@ -799,7 +789,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" ht="26.25">
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
@@ -807,7 +797,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" ht="26.25">
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
@@ -815,7 +805,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" ht="26.25">
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
@@ -823,12 +813,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -848,21 +838,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1">
       <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
@@ -879,7 +869,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="16" t="s">
         <v>21</v>
       </c>
@@ -889,119 +879,135 @@
       <c r="E2" s="14"/>
       <c r="F2" s="15"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="E4" s="7" t="s">
         <v>38</v>
       </c>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="E5" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="D6" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="E6" s="21" t="s">
         <v>38</v>
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="E7" s="22" t="s">
         <v>35</v>
       </c>
       <c r="F7" s="8"/>
       <c r="H7" s="23"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="E8" s="22" t="s">
         <v>35</v>
       </c>
       <c r="F8" s="8"/>
       <c r="H8" s="23"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="D9" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="E9" s="22" t="s">
         <v>35</v>
       </c>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="D10" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="E10" s="21" t="s">
         <v>33</v>
       </c>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+      <c r="D11" s="21" t="s">
+        <v>32</v>
+      </c>
       <c r="E11" s="21" t="s">
         <v>38</v>
       </c>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="17" t="s">
         <v>22</v>
       </c>
@@ -1011,31 +1017,35 @@
       <c r="E12" s="19"/>
       <c r="F12" s="20"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+      <c r="D13" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="E13" s="22" t="s">
         <v>35</v>
       </c>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="D14" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="E14" s="9" t="s">
         <v>35</v>
       </c>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="17" t="s">
         <v>23</v>
       </c>
@@ -1045,103 +1055,119 @@
       <c r="E15" s="19"/>
       <c r="F15" s="20"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+      <c r="D16" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="E16" s="7" t="s">
         <v>38</v>
       </c>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="D17" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="E17" s="7" t="s">
         <v>32</v>
       </c>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+      <c r="D18" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="E18" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+      <c r="D19" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="E19" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="D20" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="E20" s="9" t="s">
         <v>35</v>
       </c>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
+      <c r="D21" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="E21" s="7" t="s">
         <v>36</v>
       </c>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+      <c r="D22" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="E22" s="9" t="s">
         <v>35</v>
       </c>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+      <c r="D23" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="E23" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="17" t="s">
         <v>43</v>
       </c>
@@ -1151,43 +1177,49 @@
       <c r="E24" s="19"/>
       <c r="F24" s="20"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+      <c r="D25" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="E25" s="7" t="s">
         <v>45</v>
       </c>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="D26" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="E26" s="22" t="s">
         <v>35</v>
       </c>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+      <c r="D27" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="E27" s="21" t="s">
         <v>34</v>
       </c>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="17" t="s">
         <v>39</v>
       </c>
@@ -1197,45 +1229,49 @@
       <c r="E28" s="19"/>
       <c r="F28" s="20"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
+      <c r="D29" s="21" t="s">
+        <v>37</v>
+      </c>
       <c r="E29" s="21" t="s">
         <v>37</v>
       </c>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
+      <c r="D30" s="21" t="s">
+        <v>42</v>
+      </c>
       <c r="E30" s="21" t="s">
         <v>42</v>
       </c>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="B32" s="6"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="17" t="s">
         <v>60</v>
       </c>
@@ -1245,52 +1281,54 @@
       <c r="E33" s="19"/>
       <c r="F33" s="20"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
+      <c r="D34" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="E34" s="7" t="s">
         <v>62</v>
       </c>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="15.75" thickBot="1">
       <c r="B38" s="10"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
       <c r="F38" s="12"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="B40" s="24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="B41" s="24" t="s">
         <v>47</v>
       </c>
@@ -1298,7 +1336,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="B42" s="24" t="s">
         <v>49</v>
       </c>
@@ -1306,7 +1344,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="B43" s="24" t="s">
         <v>51</v>
       </c>
@@ -1314,7 +1352,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="B44" s="23" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
saleh has completed his skills
</commit_message>
<xml_diff>
--- a/documentation/internal/SkillsMatrix.xlsx
+++ b/documentation/internal/SkillsMatrix.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="64">
   <si>
     <t>Group 1:</t>
   </si>
@@ -466,7 +466,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="سمة Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -841,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -883,7 +883,9 @@
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
         <v>42</v>
@@ -897,7 +899,9 @@
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
         <v>35</v>
@@ -911,7 +915,9 @@
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
         <v>35</v>
@@ -925,8 +931,10 @@
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="21"/>
       <c r="D6" s="21" t="s">
         <v>35</v>
       </c>
@@ -939,7 +947,9 @@
       <c r="A7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
         <v>42</v>
@@ -954,8 +964,10 @@
       <c r="A8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="21"/>
       <c r="D8" s="7" t="s">
         <v>34</v>
       </c>
@@ -969,8 +981,10 @@
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
+      <c r="B9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="21"/>
       <c r="D9" s="21" t="s">
         <v>35</v>
       </c>
@@ -983,8 +997,10 @@
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
+      <c r="B10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="21"/>
       <c r="D10" s="7" t="s">
         <v>36</v>
       </c>
@@ -997,8 +1013,10 @@
       <c r="A11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
+      <c r="B11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="21"/>
       <c r="D11" s="21" t="s">
         <v>32</v>
       </c>
@@ -1021,8 +1039,10 @@
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
+      <c r="B13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="21"/>
       <c r="D13" s="21" t="s">
         <v>35</v>
       </c>
@@ -1035,8 +1055,10 @@
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
+      <c r="B14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="21"/>
       <c r="D14" s="21" t="s">
         <v>35</v>
       </c>
@@ -1059,8 +1081,10 @@
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
+      <c r="B16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="21"/>
       <c r="D16" s="7" t="s">
         <v>36</v>
       </c>
@@ -1073,8 +1097,10 @@
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
+      <c r="B17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="21"/>
       <c r="D17" s="7" t="s">
         <v>32</v>
       </c>
@@ -1087,8 +1113,10 @@
       <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
+      <c r="B18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="21"/>
       <c r="D18" s="7" t="s">
         <v>36</v>
       </c>
@@ -1101,8 +1129,10 @@
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
+      <c r="B19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="21"/>
       <c r="D19" s="7" t="s">
         <v>35</v>
       </c>
@@ -1115,8 +1145,10 @@
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
+      <c r="B20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="21"/>
       <c r="D20" s="21" t="s">
         <v>35</v>
       </c>
@@ -1129,8 +1161,10 @@
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
+      <c r="B21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="21"/>
       <c r="D21" s="21" t="s">
         <v>35</v>
       </c>
@@ -1143,8 +1177,10 @@
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
+      <c r="B22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="21"/>
       <c r="D22" s="21" t="s">
         <v>35</v>
       </c>
@@ -1157,8 +1193,10 @@
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
+      <c r="B23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="21"/>
       <c r="D23" s="21" t="s">
         <v>35</v>
       </c>
@@ -1181,8 +1219,10 @@
       <c r="A25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
+      <c r="B25" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="21"/>
       <c r="D25" s="7" t="s">
         <v>42</v>
       </c>
@@ -1195,8 +1235,10 @@
       <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="7"/>
+      <c r="B26" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="21"/>
       <c r="D26" s="7" t="s">
         <v>36</v>
       </c>
@@ -1209,8 +1251,10 @@
       <c r="A27" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
+      <c r="B27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="21"/>
       <c r="D27" s="7" t="s">
         <v>34</v>
       </c>
@@ -1233,8 +1277,10 @@
       <c r="A29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
+      <c r="B29" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="21"/>
       <c r="D29" s="21" t="s">
         <v>37</v>
       </c>
@@ -1247,8 +1293,10 @@
       <c r="A30" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
+      <c r="B30" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="21"/>
       <c r="D30" s="21" t="s">
         <v>42</v>
       </c>
@@ -1285,7 +1333,9 @@
       <c r="A34" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B34" s="6"/>
+      <c r="B34" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7" t="s">
         <v>32</v>

</xml_diff>